<commit_message>
Back | fix xlsx
</commit_message>
<xml_diff>
--- a/src/bin/SSS_Sofia_test2.xlsx
+++ b/src/bin/SSS_Sofia_test2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MERENKOV\Desktop\Капитан\sss\assets\fleet\9245263_sofia\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{638DC193-F43D-447C-BCE7-3A6341554FBB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC478BBE-8A6E-4420-9042-6A292C04796B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="903" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="903" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="59" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="594" uniqueCount="281">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="548" uniqueCount="267">
   <si>
     <t>Форпик</t>
   </si>
@@ -795,60 +795,6 @@
     <t>yes</t>
   </si>
   <si>
-    <t>H101</t>
-  </si>
-  <si>
-    <t>H102</t>
-  </si>
-  <si>
-    <t>H103</t>
-  </si>
-  <si>
-    <t>H104</t>
-  </si>
-  <si>
-    <t>P101</t>
-  </si>
-  <si>
-    <t>P102</t>
-  </si>
-  <si>
-    <t>P103</t>
-  </si>
-  <si>
-    <t>H201</t>
-  </si>
-  <si>
-    <t>H202</t>
-  </si>
-  <si>
-    <t>H203</t>
-  </si>
-  <si>
-    <t>H204</t>
-  </si>
-  <si>
-    <t>H205</t>
-  </si>
-  <si>
-    <t>H206</t>
-  </si>
-  <si>
-    <t>P201</t>
-  </si>
-  <si>
-    <t>P202</t>
-  </si>
-  <si>
-    <t>P203</t>
-  </si>
-  <si>
-    <t>P204</t>
-  </si>
-  <si>
-    <t>P205</t>
-  </si>
-  <si>
     <t>м∙град</t>
   </si>
   <si>
@@ -886,6 +832,18 @@
   </si>
   <si>
     <t>Поправка к поперечной метацентрической высоте</t>
+  </si>
+  <si>
+    <t>1001</t>
+  </si>
+  <si>
+    <t>Трюм №1</t>
+  </si>
+  <si>
+    <t>1002</t>
+  </si>
+  <si>
+    <t>Трюм №2</t>
   </si>
 </sst>
 </file>
@@ -986,7 +944,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2"/>
     <xf numFmtId="3" fontId="4" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyAlignment="1">
@@ -1067,6 +1025,9 @@
     </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1392,7 +1353,7 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1442,7 +1403,7 @@
       </c>
     </row>
     <row r="6" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="A6" s="29" t="s">
         <v>246</v>
       </c>
       <c r="B6" s="11" t="s">
@@ -1470,8 +1431,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1622C7A3-F812-43D4-BDBF-973F36BAE217}">
   <dimension ref="A1:L68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="E40" sqref="E40"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H62" sqref="H62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1499,21 +1460,21 @@
         <v>145</v>
       </c>
       <c r="E1" s="24" t="s">
-        <v>272</v>
+        <v>254</v>
       </c>
       <c r="F1" s="24" t="s">
-        <v>273</v>
+        <v>255</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="29" t="s">
+      <c r="A2" s="30" t="s">
         <v>211</v>
       </c>
-      <c r="B2" s="29"/>
-      <c r="C2" s="29"/>
-      <c r="D2" s="29"/>
-      <c r="E2" s="29"/>
-      <c r="F2" s="29"/>
+      <c r="B2" s="30"/>
+      <c r="C2" s="30"/>
+      <c r="D2" s="30"/>
+      <c r="E2" s="30"/>
+      <c r="F2" s="30"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="9">
@@ -1630,28 +1591,28 @@
         <v>0</v>
       </c>
       <c r="E8" s="9" t="s">
-        <v>274</v>
+        <v>256</v>
       </c>
       <c r="F8" s="9">
         <v>0.05</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="29" t="s">
+      <c r="A9" s="30" t="s">
         <v>212</v>
       </c>
-      <c r="B9" s="29"/>
-      <c r="C9" s="29"/>
-      <c r="D9" s="29"/>
-      <c r="E9" s="29"/>
-      <c r="F9" s="29"/>
+      <c r="B9" s="30"/>
+      <c r="C9" s="30"/>
+      <c r="D9" s="30"/>
+      <c r="E9" s="30"/>
+      <c r="F9" s="30"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
         <v>79</v>
       </c>
       <c r="B10" t="s">
-        <v>271</v>
+        <v>253</v>
       </c>
       <c r="C10" s="9" t="s">
         <v>148</v>
@@ -2048,14 +2009,14 @@
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" s="29" t="s">
+      <c r="A30" s="30" t="s">
         <v>213</v>
       </c>
-      <c r="B30" s="29"/>
-      <c r="C30" s="29"/>
-      <c r="D30" s="29"/>
-      <c r="E30" s="29"/>
-      <c r="F30" s="29"/>
+      <c r="B30" s="30"/>
+      <c r="C30" s="30"/>
+      <c r="D30" s="30"/>
+      <c r="E30" s="30"/>
+      <c r="F30" s="30"/>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="9" t="s">
@@ -2183,7 +2144,7 @@
         <v>92</v>
       </c>
       <c r="B37" t="s">
-        <v>269</v>
+        <v>251</v>
       </c>
       <c r="C37" s="9" t="s">
         <v>148</v>
@@ -2247,7 +2208,7 @@
         <v>95</v>
       </c>
       <c r="B40" t="s">
-        <v>270</v>
+        <v>252</v>
       </c>
       <c r="C40" s="9" t="s">
         <v>148</v>
@@ -2494,8 +2455,8 @@
       <c r="C52" s="9" t="s">
         <v>184</v>
       </c>
-      <c r="D52" s="20">
-        <v>5.1710000000000003</v>
+      <c r="D52" s="20" t="s">
+        <v>54</v>
       </c>
       <c r="E52" s="9" t="s">
         <v>54</v>
@@ -2514,8 +2475,8 @@
       <c r="C53" s="9" t="s">
         <v>184</v>
       </c>
-      <c r="D53" s="20">
-        <v>7.47</v>
+      <c r="D53" s="20" t="s">
+        <v>54</v>
       </c>
       <c r="E53" s="9" t="s">
         <v>54</v>
@@ -2758,7 +2719,7 @@
         <v>0</v>
       </c>
       <c r="E65" s="9" t="s">
-        <v>274</v>
+        <v>256</v>
       </c>
       <c r="F65" s="9">
         <v>0.05</v>
@@ -2775,7 +2736,7 @@
         <v>148</v>
       </c>
       <c r="D66" s="20">
-        <v>63.933</v>
+        <v>61.433999999999997</v>
       </c>
       <c r="E66" s="9">
         <v>1</v>
@@ -2809,7 +2770,7 @@
         <v>95</v>
       </c>
       <c r="B68" t="s">
-        <v>280</v>
+        <v>262</v>
       </c>
       <c r="C68" s="9" t="s">
         <v>148</v>
@@ -3772,10 +3733,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD512CFD-1E2E-4C9F-AF20-D54F57AEF969}">
-  <dimension ref="A1:E19"/>
+  <dimension ref="A1:O19"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D19"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J19" sqref="J19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="7.75" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3787,7 +3748,7 @@
     <col min="6" max="16384" width="7.75" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>3</v>
       </c>
@@ -3804,329 +3765,107 @@
         <v>146</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
-        <v>250</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>54</v>
+        <v>263</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>264</v>
       </c>
       <c r="C2" s="8">
-        <f>1/0.543</f>
-        <v>1.8416206261510129</v>
-      </c>
-      <c r="D2" s="5">
-        <v>900.2</v>
+        <f>1/0.54449</f>
+        <v>1.8365810207717312</v>
+      </c>
+      <c r="D2" s="3">
+        <v>3421.7</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
-        <v>254</v>
+        <v>265</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>54</v>
+        <v>266</v>
       </c>
       <c r="C3" s="8">
-        <f t="shared" ref="C3:C19" si="0">1/0.543</f>
-        <v>1.8416206261510129</v>
-      </c>
-      <c r="D3" s="5">
-        <v>51.3</v>
+        <f>1/0.54449</f>
+        <v>1.8365810207717312</v>
+      </c>
+      <c r="D3" s="3">
+        <v>4052.6</v>
       </c>
       <c r="E3" s="3" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="7" t="s">
-        <v>251</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="C4" s="8">
-        <f t="shared" si="0"/>
-        <v>1.8416206261510129</v>
-      </c>
-      <c r="D4" s="3">
-        <v>617.70000000000005</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="7" t="s">
-        <v>255</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="C5" s="8">
-        <f t="shared" si="0"/>
-        <v>1.8416206261510129</v>
-      </c>
-      <c r="D5" s="3">
-        <v>51.3</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="7" t="s">
-        <v>252</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="C6" s="8">
-        <f t="shared" si="0"/>
-        <v>1.8416206261510129</v>
-      </c>
-      <c r="D6" s="3">
-        <v>256.39999999999998</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="7" t="s">
-        <v>256</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="C7" s="8">
-        <f t="shared" si="0"/>
-        <v>1.8416206261510129</v>
-      </c>
-      <c r="D7" s="3">
-        <v>51.3</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="7" t="s">
-        <v>253</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="C8" s="8">
-        <f t="shared" si="0"/>
-        <v>1.8416206261510129</v>
-      </c>
-      <c r="D8" s="3">
-        <v>1493.5</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="7" t="s">
-        <v>257</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="C9" s="8">
-        <f t="shared" si="0"/>
-        <v>1.8416206261510129</v>
-      </c>
-      <c r="D9" s="3">
-        <v>988.3</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="7" t="s">
-        <v>263</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="C10" s="8">
-        <f t="shared" si="0"/>
-        <v>1.8416206261510129</v>
-      </c>
-      <c r="D10" s="3">
-        <v>51.3</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="7" t="s">
-        <v>258</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="C11" s="8">
-        <f t="shared" si="0"/>
-        <v>1.8416206261510129</v>
-      </c>
-      <c r="D11" s="3">
-        <v>244.5</v>
-      </c>
-      <c r="E11" s="3" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="7" t="s">
-        <v>264</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="C12" s="8">
-        <f t="shared" si="0"/>
-        <v>1.8416206261510129</v>
-      </c>
-      <c r="D12" s="3">
-        <v>51.3</v>
-      </c>
-      <c r="E12" s="3" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="7" t="s">
-        <v>259</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="C13" s="8">
-        <f t="shared" si="0"/>
-        <v>1.8416206261510129</v>
-      </c>
-      <c r="D13" s="3">
-        <v>912.7</v>
-      </c>
-      <c r="E13" s="3" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="7" t="s">
-        <v>265</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="C14" s="8">
-        <f t="shared" si="0"/>
-        <v>1.8416206261510129</v>
-      </c>
-      <c r="D14" s="3">
-        <v>51.3</v>
-      </c>
-      <c r="E14" s="3" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="7" t="s">
-        <v>260</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="C15" s="8">
-        <f t="shared" si="0"/>
-        <v>1.8416206261510129</v>
-      </c>
-      <c r="D15" s="3">
-        <v>748.7</v>
-      </c>
-      <c r="E15" s="3" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="7" t="s">
-        <v>266</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="C16" s="8">
-        <f t="shared" si="0"/>
-        <v>1.8416206261510129</v>
-      </c>
-      <c r="D16" s="3">
-        <v>51.3</v>
-      </c>
-      <c r="E16" s="3" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="7" t="s">
-        <v>261</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="C17" s="8">
-        <f t="shared" si="0"/>
-        <v>1.8416206261510129</v>
-      </c>
-      <c r="D17" s="3">
-        <v>408.6</v>
-      </c>
-      <c r="E17" s="3" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="7" t="s">
-        <v>267</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="C18" s="8">
-        <f t="shared" si="0"/>
-        <v>1.8416206261510129</v>
-      </c>
-      <c r="D18" s="3">
-        <v>51.3</v>
-      </c>
-      <c r="E18" s="3" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="7" t="s">
-        <v>262</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="C19" s="8">
-        <f t="shared" si="0"/>
-        <v>1.8416206261510129</v>
-      </c>
-      <c r="D19" s="3">
-        <v>493.3</v>
-      </c>
-      <c r="E19" s="3" t="s">
-        <v>249</v>
-      </c>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="C4" s="8"/>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="C5" s="8"/>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="C6" s="8"/>
+      <c r="J6" s="5"/>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="C7" s="8"/>
+      <c r="J7" s="5"/>
+      <c r="O7" s="3"/>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="C8" s="8"/>
+      <c r="J8" s="3"/>
+      <c r="O8" s="3"/>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="C9" s="8"/>
+      <c r="J9" s="3"/>
+      <c r="O9" s="3"/>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="C10" s="8"/>
+      <c r="J10" s="3"/>
+      <c r="O10" s="3"/>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="C11" s="8"/>
+      <c r="J11" s="3"/>
+      <c r="O11" s="3"/>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="C12" s="8"/>
+      <c r="J12" s="3"/>
+      <c r="O12" s="3"/>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="C13" s="8"/>
+      <c r="O13" s="3"/>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="C14" s="8"/>
+      <c r="O14" s="3"/>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="C15" s="8"/>
+      <c r="O15" s="3"/>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="C16" s="8"/>
+      <c r="O16" s="3"/>
+    </row>
+    <row r="17" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C17" s="8"/>
+      <c r="O17" s="3"/>
+    </row>
+    <row r="18" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C18" s="8"/>
+    </row>
+    <row r="19" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C19" s="8"/>
     </row>
   </sheetData>
   <phoneticPr fontId="5" type="noConversion"/>
@@ -4560,10 +4299,10 @@
         <v>178</v>
       </c>
       <c r="E1" s="24" t="s">
-        <v>272</v>
+        <v>254</v>
       </c>
       <c r="F1" s="24" t="s">
-        <v>273</v>
+        <v>255</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -4683,19 +4422,19 @@
         <v>176</v>
       </c>
       <c r="C1" s="25" t="s">
-        <v>275</v>
+        <v>257</v>
       </c>
       <c r="D1" s="24" t="s">
-        <v>272</v>
+        <v>254</v>
       </c>
       <c r="E1" s="24" t="s">
-        <v>273</v>
+        <v>255</v>
       </c>
       <c r="F1" s="9"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>276</v>
+        <v>258</v>
       </c>
       <c r="B2" s="9">
         <v>53.16</v>
@@ -4712,7 +4451,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>277</v>
+        <v>259</v>
       </c>
       <c r="B3" s="9">
         <v>53.16</v>
@@ -4729,7 +4468,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>278</v>
+        <v>260</v>
       </c>
       <c r="B4" s="9">
         <v>36.36</v>
@@ -4746,7 +4485,7 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>279</v>
+        <v>261</v>
       </c>
       <c r="B5" s="9">
         <v>36.36</v>
@@ -4790,10 +4529,10 @@
         <v>153</v>
       </c>
       <c r="C1" s="24" t="s">
-        <v>272</v>
+        <v>254</v>
       </c>
       <c r="D1" s="24" t="s">
-        <v>273</v>
+        <v>255</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -5100,7 +4839,7 @@
   <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+      <selection activeCell="B3" sqref="B3:D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -5127,10 +4866,10 @@
         <v>145</v>
       </c>
       <c r="E1" s="24" t="s">
-        <v>272</v>
+        <v>254</v>
       </c>
       <c r="F1" s="24" t="s">
-        <v>273</v>
+        <v>255</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -5282,7 +5021,7 @@
         <v>148</v>
       </c>
       <c r="D8" s="19">
-        <v>0.47199999999999998</v>
+        <v>0.91379999999999995</v>
       </c>
       <c r="E8" s="9">
         <v>5</v>
@@ -5397,7 +5136,7 @@
         <v>148</v>
       </c>
       <c r="D13" s="19">
-        <v>5.7099999999999998E-2</v>
+        <v>0.57099999999999995</v>
       </c>
       <c r="E13" s="9">
         <v>1</v>
@@ -5486,7 +5225,7 @@
         <v>171</v>
       </c>
       <c r="C17" s="9" t="s">
-        <v>268</v>
+        <v>250</v>
       </c>
       <c r="D17" s="19">
         <v>0.182</v>

</xml_diff>

<commit_message>
Back | change tests
</commit_message>
<xml_diff>
--- a/src/bin/SSS_Sofia_test2.xlsx
+++ b/src/bin/SSS_Sofia_test2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MERENKOV\Desktop\Капитан\sss\assets\fleet\9245263_sofia\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC478BBE-8A6E-4420-9042-6A292C04796B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E59B6F8-EBC0-4B29-A58C-5DB9E148945E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="903" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3736,7 +3736,7 @@
   <dimension ref="A1:O19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J19" sqref="J19"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="7.75" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3773,8 +3773,8 @@
         <v>264</v>
       </c>
       <c r="C2" s="8">
-        <f>1/0.54449</f>
-        <v>1.8365810207717312</v>
+        <f>1/0.543295147</f>
+        <v>1.8406201592667639</v>
       </c>
       <c r="D2" s="3">
         <v>3421.7</v>
@@ -3791,8 +3791,8 @@
         <v>266</v>
       </c>
       <c r="C3" s="8">
-        <f>1/0.54449</f>
-        <v>1.8365810207717312</v>
+        <f>1/0.543295147</f>
+        <v>1.8406201592667639</v>
       </c>
       <c r="D3" s="3">
         <v>4052.6</v>

</xml_diff>